<commit_message>
Agrega soporte para TABLE
</commit_message>
<xml_diff>
--- a/archivo.xlsx
+++ b/archivo.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Fidel\Desktop\pue\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA22A2FF-63ED-4A49-9F9C-13711F99A9C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91D16134-D919-4D98-990B-A93D8E8DEC19}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,6 +22,8 @@
     <definedName name="PUE.STRING.cadena1">Sheet1!$C$11</definedName>
     <definedName name="PUE.SWITCH.analizar">Sheet1!$D$9</definedName>
     <definedName name="PUE.SWITCH.booleanos">Sheet1!$F$9:$F$12</definedName>
+    <definedName name="PUE.TABLE.tabla_maquinas">Sheet1!$A$15:$D$18</definedName>
+    <definedName name="PUE.TABLE.tabla_xor">Sheet1!$A$20:$C$22</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -40,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
   <si>
     <t>Nombre</t>
   </si>
@@ -51,36 +53,24 @@
     <t>Edad</t>
   </si>
   <si>
-    <t>Merge</t>
-  </si>
-  <si>
     <t>Fidel</t>
   </si>
   <si>
     <t>Dalmasso</t>
   </si>
   <si>
-    <t>abc</t>
-  </si>
-  <si>
     <t>Mateo</t>
   </si>
   <si>
     <t>Toniolo</t>
   </si>
   <si>
-    <t>def</t>
-  </si>
-  <si>
     <t xml:space="preserve">Matias </t>
   </si>
   <si>
     <t>Hillar</t>
   </si>
   <si>
-    <t>ghi</t>
-  </si>
-  <si>
     <t>Suma</t>
   </si>
   <si>
@@ -112,6 +102,12 @@
   </si>
   <si>
     <t>Anios</t>
+  </si>
+  <si>
+    <t>Dato</t>
+  </si>
+  <si>
+    <t>XOR</t>
   </si>
 </sst>
 </file>
@@ -143,7 +139,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -166,24 +162,11 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -195,13 +178,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -482,10 +458,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A2:O18"/>
+  <dimension ref="A2:O22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -498,7 +474,7 @@
   <sheetData>
     <row r="2" spans="1:15" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="B2" s="4" t="s">
         <v>0</v>
@@ -509,10 +485,6 @@
       <c r="D2" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="F2" s="8"/>
       <c r="H2" s="3"/>
       <c r="M2" s="1"/>
       <c r="N2" s="3"/>
@@ -523,18 +495,14 @@
         <v>25407</v>
       </c>
       <c r="B3" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3" s="4" t="s">
         <v>4</v>
-      </c>
-      <c r="C3" s="4" t="s">
-        <v>5</v>
       </c>
       <c r="D3" s="4">
         <v>22</v>
       </c>
-      <c r="E3" s="9" t="s">
-        <v>6</v>
-      </c>
-      <c r="F3" s="8"/>
       <c r="H3" s="3"/>
       <c r="M3" s="3"/>
       <c r="N3" s="3"/>
@@ -545,18 +513,14 @@
         <v>26549</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D4" s="4">
         <v>21</v>
       </c>
-      <c r="E4" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="F4" s="8"/>
       <c r="H4" s="3"/>
       <c r="M4" s="3"/>
       <c r="N4" s="3"/>
@@ -567,18 +531,14 @@
         <v>23403</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="D5" s="4">
         <v>23</v>
       </c>
-      <c r="E5" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="F5" s="8"/>
       <c r="H5" s="3"/>
       <c r="M5" s="3"/>
       <c r="N5" s="3"/>
@@ -586,7 +546,7 @@
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.3">
       <c r="C6" s="4" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="D6" s="4">
         <f>SUM(D3:D5)</f>
@@ -603,10 +563,10 @@
     </row>
     <row r="9" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="4" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="D9" s="4" t="b">
         <v>0</v>
@@ -628,7 +588,7 @@
         <v>0.3</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="F11" s="4" t="b">
         <v>1</v>
@@ -648,20 +608,22 @@
       </c>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A15" s="5"/>
+      <c r="A15" s="5" t="s">
+        <v>20</v>
+      </c>
       <c r="B15" s="5" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="C15" s="5" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="D15" s="5" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A16" s="6" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="B16" s="6">
         <v>100</v>
@@ -675,7 +637,7 @@
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17" s="6" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="B17" s="6">
         <v>0.9</v>
@@ -689,7 +651,7 @@
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18" s="6" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="B18" s="6">
         <v>3</v>
@@ -701,13 +663,40 @@
         <v>2</v>
       </c>
     </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A20" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="B20" s="6">
+        <v>0</v>
+      </c>
+      <c r="C20" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A21" s="6">
+        <v>0</v>
+      </c>
+      <c r="B21" s="6">
+        <v>0</v>
+      </c>
+      <c r="C21" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A22" s="6">
+        <v>1</v>
+      </c>
+      <c r="B22" s="6">
+        <v>1</v>
+      </c>
+      <c r="C22" s="6">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="4">
-    <mergeCell ref="E2:F2"/>
-    <mergeCell ref="E3:F3"/>
-    <mergeCell ref="E4:F4"/>
-    <mergeCell ref="E5:F5"/>
-  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>